<commit_message>
close to creating an output. not much but its honest work
</commit_message>
<xml_diff>
--- a/student_data.xlsx
+++ b/student_data.xlsx
@@ -422,10 +422,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:I1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -435,9 +435,9 @@
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="13.140625" customWidth="1" min="5" max="5"/>
     <col width="15.140625" customWidth="1" min="6" max="6"/>
-    <col width="9.7109375" customWidth="1" min="7" max="7"/>
-    <col width="10.42578125" customWidth="1" min="8" max="8"/>
-    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="12.7109375" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="11.85546875" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -531,6 +531,241 @@
       <c r="I2" t="inlineStr">
         <is>
           <t>Fri 7:30PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Mark</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Bush</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Yellow</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1 Feb, 2022</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1 May, 2022</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Mon 3:45PM</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Tue 5:00PM</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Thu 6:00PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Nikki</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Bush</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1 Jan, 2022</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>1 Apr, 2022</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Mon 3:45PM</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Wed 6:00PM</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Hawk</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1 Jan, 2022</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>1 Jun, 2022</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Tue 6:15PM</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Thu 6:00PM</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Jill</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Brody</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1 Jan, 2022</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>1 Jun, 2022</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Tue 6:15PM</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Wed 6:00PM</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Fri 7:30PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ben</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Jamin</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1 Jan, 2022</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>1 May, 2022</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Mon 3:45PM</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Finally, there is an ouptut. Output can be sorted by belt rank or priority rating
</commit_message>
<xml_diff>
--- a/student_data.xlsx
+++ b/student_data.xlsx
@@ -422,16 +422,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.7109375" customWidth="1" min="1" max="1"/>
     <col width="14.28515625" customWidth="1" min="2" max="2"/>
+    <col width="11.7109375" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="13.140625" customWidth="1" min="5" max="5"/>
     <col width="15.140625" customWidth="1" min="6" max="6"/>
@@ -481,11 +482,7 @@
           <t>2nd Class</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>3rd Class</t>
-        </is>
-      </c>
+      <c r="I1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -520,17 +517,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Mon 3:45PM</t>
+          <t>Mon-Beg</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Tue 6:15PM</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Fri 7:30PM</t>
+          <t>Wed-Beg</t>
         </is>
       </c>
     </row>
@@ -567,17 +559,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Mon 3:45PM</t>
+          <t>Tue-Beg</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Tue 5:00PM</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Thu 6:00PM</t>
+          <t>Thu-Beg</t>
         </is>
       </c>
     </row>
@@ -614,17 +601,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Mon 3:45PM</t>
+          <t>Mon-Adv</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Wed 6:00PM</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>N/A</t>
+          <t>Wed-Adv</t>
         </is>
       </c>
     </row>
@@ -661,17 +643,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Tue 6:15PM</t>
+          <t>Mon-Adv</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Thu 6:00PM</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>N/A</t>
+          <t>Fri-Adv</t>
         </is>
       </c>
     </row>
@@ -708,17 +685,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Tue 6:15PM</t>
+          <t>Tue-Int</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Wed 6:00PM</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Fri 7:30PM</t>
+          <t>Fri-Int</t>
         </is>
       </c>
     </row>
@@ -755,17 +727,306 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Mon 3:45PM</t>
+          <t>Mon-Beg</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
+          <t>Wed-Beg</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Joe</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Mama</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>1 May, 2022</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Mon-Adv</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Tue-Adv</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Jody</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Cox</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>N/A</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>1 May, 2022</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Mon-Int</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Sat-InA</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Ben</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Harmin</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Black Stripe</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>1 May, 2022</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Mon-Adv</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Sat-InA</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Julie</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Summers</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Black Stripe</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>1 Jun, 2022</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Mon-Adv</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Sat-InA</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Lady</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Fingers</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>1 May, 2022</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Tue-Beg</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Thu-Beg</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Fat</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Buddha</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>1 May, 2022</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Tue-Int</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Fri-Int</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Evangy</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Bush</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Purple</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>1 Apr, 2022</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Mon-Adv</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Fri-Adv</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Addition of delete_student() function
</commit_message>
<xml_diff>
--- a/student_data.xlsx
+++ b/student_data.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
@@ -628,7 +628,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -670,7 +670,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -781,17 +781,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Jody</t>
+          <t>Lady</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cox</t>
+          <t>Fingers</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Orange</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -811,29 +811,29 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Mon-Int</t>
+          <t>Tue-Beg</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Sat-InA</t>
+          <t>Thu-Beg</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ben</t>
+          <t>Fat</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Harmin</t>
+          <t>Buddha</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Black Stripe</t>
+          <t>Blue</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -853,34 +853,34 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Mon-Adv</t>
+          <t>Tue-Int</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Sat-InA</t>
+          <t>Fri-Int</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Julie</t>
+          <t>Evangy</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Summers</t>
+          <t>Bush</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Black Stripe</t>
+          <t>Purple</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -890,7 +890,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>1 Jun, 2022</t>
+          <t>1 Apr, 2022</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -900,29 +900,29 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Sat-InA</t>
+          <t>Fri-Adv</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Lady</t>
+          <t>Nikki</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Fingers</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Orange</t>
+          <t>Red</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -932,101 +932,17 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>1 May, 2022</t>
+          <t>1 Jun, 2022</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Tue-Beg</t>
+          <t>Tue-Adv</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Thu-Beg</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Fat</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Buddha</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Blue</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>1 May, 2022</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Tue-Int</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Fri-Int</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Evangy</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Bush</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Purple</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>1 Apr, 2022</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Mon-Adv</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Fri-Adv</t>
+          <t>Thu-Adv</t>
         </is>
       </c>
     </row>

</xml_diff>